<commit_message>
fix template generation for datacall
</commit_message>
<xml_diff>
--- a/data/datacall_template/00template/Eel_Data_Call_Annex_Time_Series.xlsx
+++ b/data/datacall_template/00template/Eel_Data_Call_Annex_Time_Series.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="2310" windowWidth="16710" windowHeight="14370" tabRatio="851"/>
+    <workbookView xWindow="2520" yWindow="2310" windowWidth="16710" windowHeight="14370" tabRatio="851" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
@@ -5590,7 +5590,7 @@
         <xdr:cNvPr id="5" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E6B91CB-A05C-4C70-9107-EEE8E56C6F40}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5E6B91CB-A05C-4C70-9107-EEE8E56C6F40}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6836,7 +6836,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6983,7 +6983,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0A00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7082,7 +7082,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0B00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7217,7 +7217,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A342F8CB-33D0-417A-A36E-AD4A47C8FA37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A342F8CB-33D0-417A-A36E-AD4A47C8FA37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7336,7 +7336,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0C00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7459,7 +7459,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99684019-E475-4F67-BAF6-B17F21048B77}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{99684019-E475-4F67-BAF6-B17F21048B77}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7570,7 +7570,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4317529-802E-4994-BC01-27013D447207}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E4317529-802E-4994-BC01-27013D447207}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7705,7 +7705,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8959F17E-3F7A-4919-AFE3-FF3C193886E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8959F17E-3F7A-4919-AFE3-FF3C193886E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7807,7 +7807,7 @@
         <xdr:cNvPr id="2" name="Image 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF7D19C5-83A4-4758-82AA-9F9BD224E42B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EF7D19C5-83A4-4758-82AA-9F9BD224E42B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7849,7 +7849,7 @@
         <xdr:cNvPr id="2" name="Metin kutusu 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E21F326F-162D-480D-808B-0A287ADAC937}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E21F326F-162D-480D-808B-0A287ADAC937}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7904,7 +7904,7 @@
         <xdr:cNvPr id="3" name="Metin kutusu 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10B1B77D-A140-4CE5-AA2D-7105EDEB38AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{10B1B77D-A140-4CE5-AA2D-7105EDEB38AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7959,7 +7959,7 @@
         <xdr:cNvPr id="4" name="Metin kutusu 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9F3AE44-22D1-498D-AB9A-5686BF9EFA1E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E9F3AE44-22D1-498D-AB9A-5686BF9EFA1E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8014,7 +8014,7 @@
         <xdr:cNvPr id="5" name="Metin kutusu 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9B13A3C-9A80-44E0-A4A4-8766F6B6B5F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F9B13A3C-9A80-44E0-A4A4-8766F6B6B5F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8069,7 +8069,7 @@
         <xdr:cNvPr id="6" name="Metin kutusu 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D616AA12-B256-4470-86C4-F6C2C0652F50}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D616AA12-B256-4470-86C4-F6C2C0652F50}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8124,7 +8124,7 @@
         <xdr:cNvPr id="7" name="Metin kutusu 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99E8D820-DF10-4994-975A-C5CB1D4DFAA5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{99E8D820-DF10-4994-975A-C5CB1D4DFAA5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8179,7 +8179,7 @@
         <xdr:cNvPr id="8" name="Metin kutusu 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DD32F11-3437-4A9E-9D07-C160CE0311D3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DD32F11-3437-4A9E-9D07-C160CE0311D3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8234,7 +8234,7 @@
         <xdr:cNvPr id="9" name="Metin kutusu 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{840DBDDF-94F0-47B1-B461-99A7FEC8AA13}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{840DBDDF-94F0-47B1-B461-99A7FEC8AA13}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8289,7 +8289,7 @@
         <xdr:cNvPr id="10" name="Metin kutusu 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA3E0CA9-9F4B-4461-9A22-5B7C03B295BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FA3E0CA9-9F4B-4461-9A22-5B7C03B295BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8344,7 +8344,7 @@
         <xdr:cNvPr id="11" name="Metin kutusu 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1108D726-6069-41B5-BE24-4236650AFCB9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1108D726-6069-41B5-BE24-4236650AFCB9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8399,7 +8399,7 @@
         <xdr:cNvPr id="12" name="Metin kutusu 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{273D1CB8-99F4-477C-A9E9-A97BD879ABCB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{273D1CB8-99F4-477C-A9E9-A97BD879ABCB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8454,7 +8454,7 @@
         <xdr:cNvPr id="13" name="Metin kutusu 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E080288-FAE7-498D-92A0-0BA70C83D5F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0E080288-FAE7-498D-92A0-0BA70C83D5F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8509,7 +8509,7 @@
         <xdr:cNvPr id="14" name="Metin kutusu 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B78658D-5FD8-49FA-98E6-9FE2261809D1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B78658D-5FD8-49FA-98E6-9FE2261809D1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8564,7 +8564,7 @@
         <xdr:cNvPr id="15" name="Metin kutusu 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96F123D3-0ABB-4BFD-BE70-BA9AF432FF65}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{96F123D3-0ABB-4BFD-BE70-BA9AF432FF65}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8619,7 +8619,7 @@
         <xdr:cNvPr id="16" name="Metin kutusu 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC71F6CC-0F9B-45F6-8D4D-ED2DF4D20635}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AC71F6CC-0F9B-45F6-8D4D-ED2DF4D20635}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8674,7 +8674,7 @@
         <xdr:cNvPr id="17" name="Metin kutusu 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6345556C-A525-43D4-A4FD-E02BD765CF48}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6345556C-A525-43D4-A4FD-E02BD765CF48}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8729,7 +8729,7 @@
         <xdr:cNvPr id="18" name="Metin kutusu 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A5EC68C-DA9C-4939-AB23-82B3A55D0519}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3A5EC68C-DA9C-4939-AB23-82B3A55D0519}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8784,7 +8784,7 @@
         <xdr:cNvPr id="19" name="Metin kutusu 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BAC3547-7327-445E-9D58-EAFE3C92E1F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6BAC3547-7327-445E-9D58-EAFE3C92E1F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8849,7 +8849,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8950,7 +8950,7 @@
         <xdr:cNvPr id="2" name="Image 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10B44AC2-C419-43B9-86BC-FEAAC180167E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{10B44AC2-C419-43B9-86BC-FEAAC180167E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8997,7 +8997,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A17A3C2F-34EB-40E5-98D3-48A62FC2C039}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A17A3C2F-34EB-40E5-98D3-48A62FC2C039}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9040,7 +9040,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1800-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1800-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9132,7 +9132,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9305,7 +9305,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9401,7 +9401,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9493,7 +9493,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E234901-1F6D-485A-BA9A-BBF1F3770C94}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E234901-1F6D-485A-BA9A-BBF1F3770C94}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9591,7 +9591,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9691,30 +9691,24 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>363070</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>91856</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>268941</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>145678</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>290456</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>55406</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>488576</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>155763</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{176ECACF-7428-4179-8C8C-0960002D1D24}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="4" name="Image 3"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -9725,82 +9719,58 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="9354670" y="4870044"/>
-          <a:ext cx="8399033" cy="4320397"/>
+          <a:off x="8157882" y="5546913"/>
+          <a:ext cx="10058400" cy="5657850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>355066</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>358588</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>15890</xdr:rowOff>
+      <xdr:rowOff>156882</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>113864</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>212911</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>125505</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48177383-FD8F-DF19-FE59-88D94BD2A06F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="5" name="Image 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9346666" y="1889514"/>
-          <a:ext cx="7008693" cy="2679808"/>
+          <a:off x="8247529" y="1636058"/>
+          <a:ext cx="6667500" cy="3733800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9832,7 +9802,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9998,7 +9968,7 @@
         <xdr:cNvPr id="5" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92FEAA7F-4196-4D24-9292-0F040F4CEAF3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{92FEAA7F-4196-4D24-9292-0F040F4CEAF3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10072,7 +10042,7 @@
         <xdr:cNvPr id="6" name="Image 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55CBD131-7A71-495E-B9F3-AB5B4FA543DD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{55CBD131-7A71-495E-B9F3-AB5B4FA543DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10121,7 +10091,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0800-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10500,7 +10470,7 @@
   </sheetPr>
   <dimension ref="A1:AMK102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -56557,8 +56527,8 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -56757,6 +56727,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010065CE7316361DFA48AC876C6112A59FE5" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fb125599c9f9a751b726b9a94d2e235b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4d5313c0-c1e6-4122-afa9-da1ccdba405d" xmlns:ns3="362c980f-4e38-4cca-bd06-5104ee5993c5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b91c66d6a628c7b1a21e6c64315cfea9" ns2:_="" ns3:_="">
     <xsd:import namespace="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
@@ -56933,42 +56924,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD77486B-9FB1-411A-ACCC-E50815D9A26B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50425A79-54B8-4D54-9EAF-8388D1CE4120}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <ds:schemaRef ds:uri="362c980f-4e38-4cca-bd06-5104ee5993c5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -56991,9 +56950,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50425A79-54B8-4D54-9EAF-8388D1CE4120}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD77486B-9FB1-411A-ACCC-E50815D9A26B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <ds:schemaRef ds:uri="362c980f-4e38-4cca-bd06-5104ee5993c5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix heading in template
</commit_message>
<xml_diff>
--- a/data/datacall_template/00template/Eel_Data_Call_Annex_Time_Series.xlsx
+++ b/data/datacall_template/00template/Eel_Data_Call_Annex_Time_Series.xlsx
@@ -4923,13 +4923,13 @@
     <t>fi_id_cou</t>
   </si>
   <si>
-    <t>is_female(1=female,0=male)</t>
-  </si>
-  <si>
     <t>gr_lastupdate</t>
   </si>
   <si>
     <t>fi_lastupdate</t>
+  </si>
+  <si>
+    <t>is_female_(1=female,0=male)</t>
   </si>
 </sst>
 </file>
@@ -5821,7 +5821,7 @@
         <xdr:cNvPr id="5" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6972,7 +6972,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0C00-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7079,7 +7079,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0D00-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7202,7 +7202,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0E00-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7301,7 +7301,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0F00-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7436,7 +7436,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7538,7 +7538,7 @@
         <xdr:cNvPr id="2" name="Image 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7580,7 +7580,7 @@
         <xdr:cNvPr id="2" name="Metin kutusu 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7635,7 +7635,7 @@
         <xdr:cNvPr id="3" name="Metin kutusu 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7690,7 +7690,7 @@
         <xdr:cNvPr id="4" name="Metin kutusu 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7745,7 +7745,7 @@
         <xdr:cNvPr id="5" name="Metin kutusu 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7800,7 +7800,7 @@
         <xdr:cNvPr id="6" name="Metin kutusu 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7855,7 +7855,7 @@
         <xdr:cNvPr id="7" name="Metin kutusu 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7910,7 +7910,7 @@
         <xdr:cNvPr id="8" name="Metin kutusu 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7965,7 +7965,7 @@
         <xdr:cNvPr id="9" name="Metin kutusu 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8020,7 +8020,7 @@
         <xdr:cNvPr id="10" name="Metin kutusu 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8075,7 +8075,7 @@
         <xdr:cNvPr id="11" name="Metin kutusu 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8130,7 +8130,7 @@
         <xdr:cNvPr id="12" name="Metin kutusu 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8185,7 +8185,7 @@
         <xdr:cNvPr id="13" name="Metin kutusu 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8240,7 +8240,7 @@
         <xdr:cNvPr id="14" name="Metin kutusu 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8295,7 +8295,7 @@
         <xdr:cNvPr id="15" name="Metin kutusu 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-00000F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8350,7 +8350,7 @@
         <xdr:cNvPr id="16" name="Metin kutusu 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-000010000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8405,7 +8405,7 @@
         <xdr:cNvPr id="17" name="Metin kutusu 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-000011000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8460,7 +8460,7 @@
         <xdr:cNvPr id="18" name="Metin kutusu 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-000012000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8515,7 +8515,7 @@
         <xdr:cNvPr id="19" name="Metin kutusu 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1200-000013000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8575,7 +8575,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1A00-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1A00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8667,7 +8667,7 @@
         <xdr:cNvPr id="2" name="Image 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1800-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1800-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8714,7 +8714,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1900-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1900-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8762,7 +8762,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8935,7 +8935,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9033,7 +9033,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9151,7 +9151,7 @@
         <xdr:cNvPr id="4" name="Image 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9201,7 +9201,7 @@
         <xdr:cNvPr id="5" name="Image 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9256,7 +9256,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9422,7 +9422,7 @@
         <xdr:cNvPr id="7" name="Image 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9472,7 +9472,7 @@
         <xdr:cNvPr id="8" name="Image 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9527,7 +9527,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0800-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9634,7 +9634,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9757,7 +9757,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0A00-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9856,7 +9856,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0B00-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10580,7 +10580,7 @@
     </row>
     <row r="41" spans="1:5 1025:1025">
       <c r="A41" s="54" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="B41" s="47" t="s">
         <v>1281</v>
@@ -10847,7 +10847,7 @@
     </row>
     <row r="71" spans="1:2 1025:1025">
       <c r="A71" s="54" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="B71" s="47" t="s">
         <v>1281</v>
@@ -10903,7 +10903,7 @@
     </row>
     <row r="78" spans="1:2 1025:1025">
       <c r="A78" s="61" t="s">
-        <v>1552</v>
+        <v>1554</v>
       </c>
       <c r="B78" s="62" t="s">
         <v>1300</v>
@@ -11030,7 +11030,7 @@
         <v>1237</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="G1" s="34" t="s">
         <v>1238</v>
@@ -11215,7 +11215,7 @@
         <v>1242</v>
       </c>
       <c r="H1" s="33" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="I1" s="33" t="s">
         <v>1243</v>
@@ -11236,7 +11236,7 @@
         <v>1197</v>
       </c>
       <c r="O1" s="70" t="s">
-        <v>1552</v>
+        <v>1554</v>
       </c>
       <c r="P1" s="38" t="s">
         <v>1520</v>
@@ -11330,7 +11330,7 @@
         <v>1197</v>
       </c>
       <c r="L1" s="70" t="s">
-        <v>1552</v>
+        <v>1554</v>
       </c>
       <c r="M1" s="38" t="s">
         <v>1520</v>
@@ -11443,7 +11443,7 @@
         <v>1242</v>
       </c>
       <c r="H1" s="33" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="I1" s="38" t="s">
         <v>1243</v>
@@ -11464,7 +11464,7 @@
         <v>1197</v>
       </c>
       <c r="O1" s="70" t="s">
-        <v>1552</v>
+        <v>1554</v>
       </c>
       <c r="P1" s="38" t="s">
         <v>1520</v>
@@ -11576,7 +11576,7 @@
         <v>1242</v>
       </c>
       <c r="H1" s="33" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="I1" s="38" t="s">
         <v>1243</v>
@@ -11597,7 +11597,7 @@
         <v>1197</v>
       </c>
       <c r="O1" s="70" t="s">
-        <v>1552</v>
+        <v>1554</v>
       </c>
       <c r="P1" s="38" t="s">
         <v>1520</v>
@@ -13640,7 +13640,7 @@
         <v>1226</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>1552</v>
+        <v>1554</v>
       </c>
       <c r="D7" s="42" t="s">
         <v>1257</v>
@@ -31945,7 +31945,7 @@
         <v>1237</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="G1" s="33" t="s">
         <v>1238</v>
@@ -49847,7 +49847,7 @@
         <v>1237</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="G1" s="33" t="s">
         <v>1238</v>
@@ -50051,6 +50051,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ADE5A2812409A74E9D63F27EF88903B8" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7bd325d4d8d3d0cfa3a820f8985111cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4d5313c0-c1e6-4122-afa9-da1ccdba405d" xmlns:ns3="362c980f-4e38-4cca-bd06-5104ee5993c5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a46f65cc92525120babafc4c69c5d04c" ns2:_="" ns3:_="">
     <xsd:import namespace="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
@@ -50227,18 +50239,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -50249,6 +50249,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26A31DF9-0697-482A-AA13-03351BA7D829}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="362c980f-4e38-4cca-bd06-5104ee5993c5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F5E65C0-0531-4AD3-8512-1785183D40D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -50267,23 +50284,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26A31DF9-0697-482A-AA13-03351BA7D829}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="362c980f-4e38-4cca-bd06-5104ee5993c5"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50425A79-54B8-4D54-9EAF-8388D1CE4120}">
   <ds:schemaRefs>

</xml_diff>